<commit_message>
End of thursd b4 dchmp
</commit_message>
<xml_diff>
--- a/ROBOT_CODE/AlexanderGCowbell/src/main/java/frc/data/mp/SmoothedPaths.xlsx
+++ b/ROBOT_CODE/AlexanderGCowbell/src/main/java/frc/data/mp/SmoothedPaths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SHARED\FRC2023\ROBOT_CODE\AlexanderGCowbell\src\main\java\frc\data\mp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FCEF30-70C7-4106-AAC2-3FB0454FCA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF0DB51-A410-4A1F-8ADE-F8186774BF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1710" yWindow="0" windowWidth="18900" windowHeight="14895" tabRatio="1000" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScoreConeHigh" sheetId="3" r:id="rId1"/>
@@ -8468,8 +8468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752DA2FE-56D1-4F82-A910-2BE20092F8F9}">
   <dimension ref="A1:V280"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" topLeftCell="G39" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8626,11 +8626,11 @@
       </c>
       <c r="N3">
         <f t="shared" ref="N3:O18" si="3">H3+U$9 +($M2*U$10)</f>
-        <v>-4558.5476190476193</v>
+        <v>-4418.7083333333339</v>
       </c>
       <c r="O3">
         <f t="shared" si="3"/>
-        <v>10355.101190476191</v>
+        <v>10355.29761904762</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:Q58" si="4">J3</f>
@@ -8691,11 +8691,11 @@
       </c>
       <c r="N4">
         <f t="shared" si="3"/>
-        <v>-4640.0285714285719</v>
+        <v>-4360.3500000000004</v>
       </c>
       <c r="O4">
         <f t="shared" si="3"/>
-        <v>10372.335714285713</v>
+        <v>10372.72857142857</v>
       </c>
       <c r="P4">
         <f t="shared" si="4"/>
@@ -8713,10 +8713,10 @@
         <v>8</v>
       </c>
       <c r="U4" s="2">
-        <v>-8000</v>
+        <v>-169</v>
       </c>
       <c r="V4" s="3">
-        <v>20000</v>
+        <v>20011</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -8756,11 +8756,11 @@
       </c>
       <c r="N5">
         <f t="shared" si="3"/>
-        <v>-4742.6428571428569</v>
+        <v>-4323.125</v>
       </c>
       <c r="O5">
         <f t="shared" si="3"/>
-        <v>10438.503571428571</v>
+        <v>10439.092857142858</v>
       </c>
       <c r="P5">
         <f t="shared" si="4"/>
@@ -8823,11 +8823,11 @@
       </c>
       <c r="N6">
         <f t="shared" si="3"/>
-        <v>-4811.8571428571431</v>
+        <v>-4252.5</v>
       </c>
       <c r="O6">
         <f t="shared" si="3"/>
-        <v>10490.471428571429</v>
+        <v>10491.257142857143</v>
       </c>
       <c r="P6">
         <f t="shared" si="4"/>
@@ -8890,11 +8890,11 @@
       </c>
       <c r="N7">
         <f t="shared" si="3"/>
-        <v>-4889.0714285714284</v>
+        <v>-4189.875</v>
       </c>
       <c r="O7">
         <f t="shared" si="3"/>
-        <v>10614.839285714286</v>
+        <v>10615.821428571429</v>
       </c>
       <c r="P7">
         <f t="shared" si="4"/>
@@ -8957,11 +8957,11 @@
       </c>
       <c r="N8">
         <f t="shared" si="3"/>
-        <v>-4966.2857142857147</v>
+        <v>-4127.25</v>
       </c>
       <c r="O8">
         <f t="shared" si="3"/>
-        <v>10739.207142857143</v>
+        <v>10740.385714285714</v>
       </c>
       <c r="P8">
         <f t="shared" si="4"/>
@@ -9013,11 +9013,11 @@
       </c>
       <c r="N9">
         <f t="shared" si="3"/>
-        <v>-5043.5</v>
+        <v>-4064.625</v>
       </c>
       <c r="O9">
         <f t="shared" si="3"/>
-        <v>10863.575000000001</v>
+        <v>10864.95</v>
       </c>
       <c r="P9">
         <f t="shared" si="4"/>
@@ -9080,11 +9080,11 @@
       </c>
       <c r="N10">
         <f t="shared" si="3"/>
-        <v>-5112.3142857142857</v>
+        <v>-3993.6000000000004</v>
       </c>
       <c r="O10">
         <f t="shared" si="3"/>
-        <v>11029.342857142858</v>
+        <v>11030.914285714287</v>
       </c>
       <c r="P10">
         <f t="shared" si="4"/>
@@ -9103,11 +9103,11 @@
       </c>
       <c r="U10">
         <f>(U4-U6-U9)/(U7-1)</f>
-        <v>-59.214285714285715</v>
+        <v>80.625</v>
       </c>
       <c r="V10">
         <f>(V4-V6-V9)/(V7-1)</f>
-        <v>7.7678571428571432</v>
+        <v>7.9642857142857144</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -9147,11 +9147,11 @@
       </c>
       <c r="N11">
         <f t="shared" si="3"/>
-        <v>-5181.1285714285723</v>
+        <v>-3922.5750000000007</v>
       </c>
       <c r="O11">
         <f t="shared" si="3"/>
-        <v>11195.110714285714</v>
+        <v>11196.878571428571</v>
       </c>
       <c r="P11">
         <f t="shared" si="4"/>
@@ -9203,11 +9203,11 @@
       </c>
       <c r="N12">
         <f t="shared" si="3"/>
-        <v>-5241.9428571428562</v>
+        <v>-3843.5499999999993</v>
       </c>
       <c r="O12">
         <f t="shared" si="3"/>
-        <v>11378.878571428571</v>
+        <v>11380.842857142858</v>
       </c>
       <c r="P12">
         <f t="shared" si="4"/>
@@ -9259,11 +9259,11 @@
       </c>
       <c r="N13">
         <f t="shared" si="3"/>
-        <v>-5299.3571428571431</v>
+        <v>-3761.125</v>
       </c>
       <c r="O13">
         <f t="shared" si="3"/>
-        <v>11562.64642857143</v>
+        <v>11564.807142857144</v>
       </c>
       <c r="P13">
         <f t="shared" si="4"/>
@@ -9315,11 +9315,11 @@
       </c>
       <c r="N14">
         <f t="shared" si="3"/>
-        <v>-5357.3714285714277</v>
+        <v>-3679.2999999999993</v>
       </c>
       <c r="O14">
         <f t="shared" si="3"/>
-        <v>11842.814285714287</v>
+        <v>11845.17142857143</v>
       </c>
       <c r="P14">
         <f t="shared" si="4"/>
@@ -9371,11 +9371,11 @@
       </c>
       <c r="N15">
         <f t="shared" si="3"/>
-        <v>-5413.7857142857147</v>
+        <v>-3595.875</v>
       </c>
       <c r="O15">
         <f t="shared" si="3"/>
-        <v>12037.382142857143</v>
+        <v>12039.935714285713</v>
       </c>
       <c r="P15">
         <f t="shared" si="4"/>
@@ -9427,11 +9427,11 @@
       </c>
       <c r="N16">
         <f t="shared" si="3"/>
-        <v>-5470.2000000000007</v>
+        <v>-3512.4500000000007</v>
       </c>
       <c r="O16">
         <f t="shared" si="3"/>
-        <v>12337.35</v>
+        <v>12340.1</v>
       </c>
       <c r="P16">
         <f t="shared" si="4"/>
@@ -9483,11 +9483,11 @@
       </c>
       <c r="N17">
         <f t="shared" si="3"/>
-        <v>-5526.6142857142859</v>
+        <v>-3429.0249999999996</v>
       </c>
       <c r="O17">
         <f t="shared" si="3"/>
-        <v>12546.917857142857</v>
+        <v>12549.864285714286</v>
       </c>
       <c r="P17">
         <f t="shared" si="4"/>
@@ -9539,11 +9539,11 @@
       </c>
       <c r="N18">
         <f t="shared" si="3"/>
-        <v>-5586.4285714285716</v>
+        <v>-3349</v>
       </c>
       <c r="O18">
         <f t="shared" si="3"/>
-        <v>12756.485714285714</v>
+        <v>12759.628571428571</v>
       </c>
       <c r="P18">
         <f t="shared" si="4"/>
@@ -9595,11 +9595,11 @@
       </c>
       <c r="N19">
         <f t="shared" ref="N19:O34" si="7">H19+U$9 +($M18*U$10)</f>
-        <v>-5645.6428571428569</v>
+        <v>-3268.375</v>
       </c>
       <c r="O19">
         <f t="shared" si="7"/>
-        <v>12985.053571428571</v>
+        <v>12988.392857142857</v>
       </c>
       <c r="P19">
         <f t="shared" si="4"/>
@@ -9651,11 +9651,11 @@
       </c>
       <c r="N20">
         <f t="shared" si="7"/>
-        <v>-5704.8571428571431</v>
+        <v>-3187.75</v>
       </c>
       <c r="O20">
         <f t="shared" si="7"/>
-        <v>13213.621428571429</v>
+        <v>13217.157142857142</v>
       </c>
       <c r="P20">
         <f t="shared" si="4"/>
@@ -9707,11 +9707,11 @@
       </c>
       <c r="N21">
         <f t="shared" si="7"/>
-        <v>-5764.0714285714284</v>
+        <v>-3107.125</v>
       </c>
       <c r="O21">
         <f t="shared" si="7"/>
-        <v>13452.789285714287</v>
+        <v>13456.52142857143</v>
       </c>
       <c r="P21">
         <f t="shared" si="4"/>
@@ -9763,11 +9763,11 @@
       </c>
       <c r="N22">
         <f t="shared" si="7"/>
-        <v>-5823.2857142857138</v>
+        <v>-3026.5</v>
       </c>
       <c r="O22">
         <f t="shared" si="7"/>
-        <v>13691.957142857143</v>
+        <v>13695.885714285714</v>
       </c>
       <c r="P22">
         <f t="shared" si="4"/>
@@ -9819,11 +9819,11 @@
       </c>
       <c r="N23">
         <f t="shared" si="7"/>
-        <v>-5883.2999999999993</v>
+        <v>-2946.6749999999993</v>
       </c>
       <c r="O23">
         <f t="shared" si="7"/>
-        <v>14042.125</v>
+        <v>14046.25</v>
       </c>
       <c r="P23">
         <f t="shared" si="4"/>
@@ -9875,11 +9875,11 @@
       </c>
       <c r="N24">
         <f t="shared" si="7"/>
-        <v>-5943.3142857142866</v>
+        <v>-2866.8500000000004</v>
       </c>
       <c r="O24">
         <f t="shared" si="7"/>
-        <v>14276.892857142857</v>
+        <v>14281.214285714286</v>
       </c>
       <c r="P24">
         <f t="shared" si="4"/>
@@ -9931,11 +9931,11 @@
       </c>
       <c r="N25">
         <f t="shared" si="7"/>
-        <v>-6007.1285714285723</v>
+        <v>-2790.8250000000007</v>
       </c>
       <c r="O25">
         <f t="shared" si="7"/>
-        <v>14616.460714285713</v>
+        <v>14620.97857142857</v>
       </c>
       <c r="P25">
         <f t="shared" si="4"/>
@@ -9987,11 +9987,11 @@
       </c>
       <c r="N26">
         <f t="shared" si="7"/>
-        <v>-6070.9428571428562</v>
+        <v>-2714.7999999999993</v>
       </c>
       <c r="O26">
         <f t="shared" si="7"/>
-        <v>14840.028571428569</v>
+        <v>14844.742857142855</v>
       </c>
       <c r="P26">
         <f t="shared" si="4"/>
@@ -10043,11 +10043,11 @@
       </c>
       <c r="N27">
         <f t="shared" si="7"/>
-        <v>-6139.5571428571438</v>
+        <v>-2643.5750000000007</v>
       </c>
       <c r="O27">
         <f t="shared" si="7"/>
-        <v>15160.996428571429</v>
+        <v>15165.907142857142</v>
       </c>
       <c r="P27">
         <f t="shared" si="4"/>
@@ -10099,11 +10099,11 @@
       </c>
       <c r="N28">
         <f t="shared" si="7"/>
-        <v>-6207.3714285714277</v>
+        <v>-2571.5499999999993</v>
       </c>
       <c r="O28">
         <f t="shared" si="7"/>
-        <v>15370.964285714286</v>
+        <v>15376.071428571429</v>
       </c>
       <c r="P28">
         <f t="shared" si="4"/>
@@ -10155,11 +10155,11 @@
       </c>
       <c r="N29">
         <f t="shared" si="7"/>
-        <v>-6275.1857142857134</v>
+        <v>-2499.5249999999996</v>
       </c>
       <c r="O29">
         <f t="shared" si="7"/>
-        <v>15671.932142857144</v>
+        <v>15677.235714285714</v>
       </c>
       <c r="P29">
         <f t="shared" si="4"/>
@@ -10211,11 +10211,11 @@
       </c>
       <c r="N30">
         <f t="shared" si="7"/>
-        <v>-6339.2000000000007</v>
+        <v>-2423.7000000000007</v>
       </c>
       <c r="O30">
         <f t="shared" si="7"/>
-        <v>15868.099999999999</v>
+        <v>15873.599999999999</v>
       </c>
       <c r="P30">
         <f t="shared" si="4"/>
@@ -10267,11 +10267,11 @@
       </c>
       <c r="N31">
         <f t="shared" si="7"/>
-        <v>-6403.0142857142855</v>
+        <v>-2347.6749999999993</v>
       </c>
       <c r="O31">
         <f t="shared" si="7"/>
-        <v>16235.067857142856</v>
+        <v>16240.764285714286</v>
       </c>
       <c r="P31">
         <f t="shared" si="4"/>
@@ -10323,11 +10323,11 @@
       </c>
       <c r="N32">
         <f t="shared" si="7"/>
-        <v>-6462.0285714285719</v>
+        <v>-2266.8500000000004</v>
       </c>
       <c r="O32">
         <f t="shared" si="7"/>
-        <v>16504.635714285712</v>
+        <v>16510.528571428571</v>
       </c>
       <c r="P32">
         <f t="shared" si="4"/>
@@ -10379,11 +10379,11 @@
       </c>
       <c r="N33">
         <f t="shared" si="7"/>
-        <v>-6520.8428571428576</v>
+        <v>-2185.8250000000007</v>
       </c>
       <c r="O33">
         <f t="shared" si="7"/>
-        <v>16859.803571428572</v>
+        <v>16865.892857142859</v>
       </c>
       <c r="P33">
         <f t="shared" si="4"/>
@@ -10435,11 +10435,11 @@
       </c>
       <c r="N34">
         <f t="shared" si="7"/>
-        <v>-6579.6571428571424</v>
+        <v>-2104.7999999999993</v>
       </c>
       <c r="O34">
         <f t="shared" si="7"/>
-        <v>17123.971428571429</v>
+        <v>17130.257142857143</v>
       </c>
       <c r="P34">
         <f t="shared" si="4"/>
@@ -10491,11 +10491,11 @@
       </c>
       <c r="N35">
         <f t="shared" ref="N35:O50" si="9">H35+U$9 +($M34*U$10)</f>
-        <v>-6638.4714285714281</v>
+        <v>-2023.7749999999996</v>
       </c>
       <c r="O35">
         <f t="shared" si="9"/>
-        <v>17388.139285714286</v>
+        <v>17394.621428571427</v>
       </c>
       <c r="P35">
         <f t="shared" si="4"/>
@@ -10547,11 +10547,11 @@
       </c>
       <c r="N36">
         <f t="shared" si="9"/>
-        <v>-6697.4857142857145</v>
+        <v>-1942.9500000000007</v>
       </c>
       <c r="O36">
         <f t="shared" si="9"/>
-        <v>17563.70714285714</v>
+        <v>17570.385714285712</v>
       </c>
       <c r="P36">
         <f t="shared" si="4"/>
@@ -10603,11 +10603,11 @@
       </c>
       <c r="N37">
         <f t="shared" si="9"/>
-        <v>-6756.5</v>
+        <v>-1862.125</v>
       </c>
       <c r="O37">
         <f t="shared" si="9"/>
-        <v>17739.275000000001</v>
+        <v>17746.150000000001</v>
       </c>
       <c r="P37">
         <f t="shared" si="4"/>
@@ -10659,11 +10659,11 @@
       </c>
       <c r="N38">
         <f t="shared" si="9"/>
-        <v>-6815.7142857142862</v>
+        <v>-1781.5</v>
       </c>
       <c r="O38">
         <f t="shared" si="9"/>
-        <v>17904.242857142857</v>
+        <v>17911.314285714285</v>
       </c>
       <c r="P38">
         <f t="shared" si="4"/>
@@ -10715,11 +10715,11 @@
       </c>
       <c r="N39">
         <f t="shared" si="9"/>
-        <v>-6874.9285714285716</v>
+        <v>-1700.875</v>
       </c>
       <c r="O39">
         <f t="shared" si="9"/>
-        <v>18069.210714285713</v>
+        <v>18076.478571428572</v>
       </c>
       <c r="P39">
         <f t="shared" si="4"/>
@@ -10771,11 +10771,11 @@
       </c>
       <c r="N40">
         <f t="shared" si="9"/>
-        <v>-6934.1428571428569</v>
+        <v>-1620.25</v>
       </c>
       <c r="O40">
         <f t="shared" si="9"/>
-        <v>18301.778571428571</v>
+        <v>18309.242857142857</v>
       </c>
       <c r="P40">
         <f t="shared" si="4"/>
@@ -10827,11 +10827,11 @@
       </c>
       <c r="N41">
         <f t="shared" si="9"/>
-        <v>-6993.3571428571431</v>
+        <v>-1539.625</v>
       </c>
       <c r="O41">
         <f t="shared" si="9"/>
-        <v>18452.146428571428</v>
+        <v>18459.807142857142</v>
       </c>
       <c r="P41">
         <f t="shared" si="4"/>
@@ -10883,11 +10883,11 @@
       </c>
       <c r="N42">
         <f t="shared" si="9"/>
-        <v>-7052.5714285714284</v>
+        <v>-1459</v>
       </c>
       <c r="O42">
         <f t="shared" si="9"/>
-        <v>18661.314285714285</v>
+        <v>18669.171428571426</v>
       </c>
       <c r="P42">
         <f t="shared" si="4"/>
@@ -10939,11 +10939,11 @@
       </c>
       <c r="N43">
         <f t="shared" si="9"/>
-        <v>-7111.7857142857138</v>
+        <v>-1378.375</v>
       </c>
       <c r="O43">
         <f t="shared" si="9"/>
-        <v>18795.482142857141</v>
+        <v>18803.535714285714</v>
       </c>
       <c r="P43">
         <f t="shared" si="4"/>
@@ -10995,11 +10995,11 @@
       </c>
       <c r="N44">
         <f t="shared" si="9"/>
-        <v>-7171</v>
+        <v>-1297.75</v>
       </c>
       <c r="O44">
         <f t="shared" si="9"/>
-        <v>18978.45</v>
+        <v>18986.7</v>
       </c>
       <c r="P44">
         <f t="shared" si="4"/>
@@ -11051,11 +11051,11 @@
       </c>
       <c r="N45">
         <f t="shared" si="9"/>
-        <v>-7230.2142857142862</v>
+        <v>-1217.125</v>
       </c>
       <c r="O45">
         <f t="shared" si="9"/>
-        <v>19093.817857142858</v>
+        <v>19102.264285714286</v>
       </c>
       <c r="P45">
         <f t="shared" si="4"/>
@@ -11107,11 +11107,11 @@
       </c>
       <c r="N46">
         <f t="shared" si="9"/>
-        <v>-7289.4285714285716</v>
+        <v>-1136.5</v>
       </c>
       <c r="O46">
         <f t="shared" si="9"/>
-        <v>19249.185714285715</v>
+        <v>19257.828571428574</v>
       </c>
       <c r="P46">
         <f t="shared" si="4"/>
@@ -11163,11 +11163,11 @@
       </c>
       <c r="N47">
         <f t="shared" si="9"/>
-        <v>-7348.6428571428569</v>
+        <v>-1055.875</v>
       </c>
       <c r="O47">
         <f t="shared" si="9"/>
-        <v>19345.753571428573</v>
+        <v>19354.592857142859</v>
       </c>
       <c r="P47">
         <f t="shared" si="4"/>
@@ -11219,11 +11219,11 @@
       </c>
       <c r="N48">
         <f t="shared" si="9"/>
-        <v>-7407.8571428571431</v>
+        <v>-975.25</v>
       </c>
       <c r="O48">
         <f t="shared" si="9"/>
-        <v>19474.121428571427</v>
+        <v>19483.157142857141</v>
       </c>
       <c r="P48">
         <f t="shared" si="4"/>
@@ -11275,11 +11275,11 @@
       </c>
       <c r="N49">
         <f t="shared" si="9"/>
-        <v>-7467.0714285714284</v>
+        <v>-894.625</v>
       </c>
       <c r="O49">
         <f t="shared" si="9"/>
-        <v>19553.689285714285</v>
+        <v>19562.921428571426</v>
       </c>
       <c r="P49">
         <f t="shared" si="4"/>
@@ -11331,11 +11331,11 @@
       </c>
       <c r="N50">
         <f t="shared" si="9"/>
-        <v>-7526.2857142857138</v>
+        <v>-814</v>
       </c>
       <c r="O50">
         <f t="shared" si="9"/>
-        <v>19657.657142857141</v>
+        <v>19667.085714285713</v>
       </c>
       <c r="P50">
         <f t="shared" si="4"/>
@@ -11387,11 +11387,11 @@
       </c>
       <c r="N51">
         <f t="shared" ref="N51:O58" si="11">H51+U$9 +($M50*U$10)</f>
-        <v>-7585.5</v>
+        <v>-733.375</v>
       </c>
       <c r="O51">
         <f t="shared" si="11"/>
-        <v>19721.625</v>
+        <v>19731.25</v>
       </c>
       <c r="P51">
         <f t="shared" si="4"/>
@@ -11443,11 +11443,11 @@
       </c>
       <c r="N52">
         <f t="shared" si="11"/>
-        <v>-7644.7142857142862</v>
+        <v>-652.75</v>
       </c>
       <c r="O52">
         <f t="shared" si="11"/>
-        <v>19802.79285714286</v>
+        <v>19812.614285714288</v>
       </c>
       <c r="P52">
         <f t="shared" si="4"/>
@@ -11499,11 +11499,11 @@
       </c>
       <c r="N53">
         <f t="shared" si="11"/>
-        <v>-7703.9285714285716</v>
+        <v>-572.125</v>
       </c>
       <c r="O53">
         <f t="shared" si="11"/>
-        <v>19852.160714285714</v>
+        <v>19862.178571428572</v>
       </c>
       <c r="P53">
         <f t="shared" si="4"/>
@@ -11555,11 +11555,11 @@
       </c>
       <c r="N54">
         <f t="shared" si="11"/>
-        <v>-7763.1428571428569</v>
+        <v>-491.5</v>
       </c>
       <c r="O54">
         <f t="shared" si="11"/>
-        <v>19909.128571428573</v>
+        <v>19919.342857142859</v>
       </c>
       <c r="P54">
         <f t="shared" si="4"/>
@@ -11611,11 +11611,11 @@
       </c>
       <c r="N55">
         <f t="shared" si="11"/>
-        <v>-7822.3571428571431</v>
+        <v>-410.875</v>
       </c>
       <c r="O55">
         <f t="shared" si="11"/>
-        <v>19941.696428571428</v>
+        <v>19952.107142857141</v>
       </c>
       <c r="P55">
         <f t="shared" si="4"/>
@@ -11667,11 +11667,11 @@
       </c>
       <c r="N56">
         <f t="shared" si="11"/>
-        <v>-7881.5714285714284</v>
+        <v>-330.25</v>
       </c>
       <c r="O56">
         <f t="shared" si="11"/>
-        <v>19973.264285714286</v>
+        <v>19983.871428571427</v>
       </c>
       <c r="P56">
         <f t="shared" si="4"/>
@@ -11723,11 +11723,11 @@
       </c>
       <c r="N57">
         <f t="shared" si="11"/>
-        <v>-7940.7857142857138</v>
+        <v>-249.625</v>
       </c>
       <c r="O57">
         <f t="shared" si="11"/>
-        <v>19995.565476190473</v>
+        <v>20006.369047619046</v>
       </c>
       <c r="P57">
         <f t="shared" si="4"/>
@@ -11779,11 +11779,11 @@
       </c>
       <c r="N58">
         <f t="shared" si="11"/>
-        <v>-8000</v>
+        <v>-169</v>
       </c>
       <c r="O58">
         <f t="shared" si="11"/>
-        <v>20000</v>
+        <v>20011</v>
       </c>
       <c r="P58">
         <f t="shared" si="4"/>
@@ -27604,7 +27604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3ECCBA-6D4F-466F-804D-502AE8BB8A06}">
   <dimension ref="A1:V331"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N1" sqref="N1:R1048576"/>
     </sheetView>
   </sheetViews>
@@ -33303,7 +33303,7 @@
         <v>0.114246308803558</v>
       </c>
       <c r="H101">
-        <f t="shared" ref="H101:K105" si="20">AVERAGE(A99:A103)</f>
+        <f t="shared" ref="H101:K104" si="20">AVERAGE(A99:A103)</f>
         <v>-27226.400000000001</v>
       </c>
       <c r="I101">

</xml_diff>

<commit_message>
fix cone scoring in auto - verified in practice area
</commit_message>
<xml_diff>
--- a/ROBOT_CODE/AlexanderGCowbell/src/main/java/frc/data/mp/SmoothedPaths.xlsx
+++ b/ROBOT_CODE/AlexanderGCowbell/src/main/java/frc/data/mp/SmoothedPaths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SHARED\FRC2023\ROBOT_CODE\AlexanderGCowbell\src\main\java\frc\data\mp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D913ACA-A7FD-4BAB-BB05-2FEAD1727CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E6256F-D1F1-4868-B2A3-FE79EA9C0FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScoreConeHigh" sheetId="3" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="17">
   <si>
     <t>proximal_pos</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Pic</t>
+  </si>
+  <si>
+    <t>was</t>
+  </si>
+  <si>
+    <t>proximal</t>
   </si>
 </sst>
 </file>
@@ -12916,9 +12922,9 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8F3C61-007F-4AD8-A4FD-90C2D7D20C99}">
-  <dimension ref="A1:V340"/>
+  <dimension ref="A1:Y340"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:R1048576"/>
     </sheetView>
   </sheetViews>
@@ -12929,7 +12935,7 @@
     <col min="22" max="22" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12977,7 +12983,7 @@
         <v xml:space="preserve"> wrist_pos</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-9022</v>
       </c>
@@ -13038,8 +13044,11 @@
       <c r="V2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>-9022</v>
       </c>
@@ -13076,7 +13085,7 @@
       </c>
       <c r="N3">
         <f t="shared" ref="N3:O18" si="3">H3+U$9 +($M2*U$10)</f>
-        <v>-4462.2181818181816</v>
+        <v>-4498.5818181818186</v>
       </c>
       <c r="O3">
         <f t="shared" si="3"/>
@@ -13103,8 +13112,11 @@
       <c r="V3">
         <v>10300</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>-9022</v>
       </c>
@@ -13141,7 +13153,7 @@
       </c>
       <c r="N4">
         <f t="shared" si="3"/>
-        <v>-4587.8363636363629</v>
+        <v>-4660.5636363636359</v>
       </c>
       <c r="O4">
         <f t="shared" si="3"/>
@@ -13163,13 +13175,16 @@
         <v>8</v>
       </c>
       <c r="U4" s="2">
-        <v>-45000</v>
+        <v>-49000</v>
       </c>
       <c r="V4" s="3">
         <v>-50000</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Y4">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-9022</v>
       </c>
@@ -13206,7 +13221,7 @@
       </c>
       <c r="N5">
         <f t="shared" si="3"/>
-        <v>-4713.454545454545</v>
+        <v>-4822.545454545454</v>
       </c>
       <c r="O5">
         <f t="shared" si="3"/>
@@ -13236,7 +13251,7 @@
         <v>7122</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-9279</v>
       </c>
@@ -13273,7 +13288,7 @@
       </c>
       <c r="N6">
         <f t="shared" si="3"/>
-        <v>-4904.4727272727278</v>
+        <v>-5049.9272727272728</v>
       </c>
       <c r="O6">
         <f t="shared" si="3"/>
@@ -13303,7 +13318,7 @@
         <v>-53408</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-9279</v>
       </c>
@@ -13340,7 +13355,7 @@
       </c>
       <c r="N7">
         <f t="shared" si="3"/>
-        <v>-5095.4909090909086</v>
+        <v>-5277.3090909090906</v>
       </c>
       <c r="O7">
         <f t="shared" si="3"/>
@@ -13370,7 +13385,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-9606</v>
       </c>
@@ -13407,7 +13422,7 @@
       </c>
       <c r="N8">
         <f t="shared" si="3"/>
-        <v>-5348.5090909090914</v>
+        <v>-5566.6909090909103</v>
       </c>
       <c r="O8">
         <f t="shared" si="3"/>
@@ -13426,7 +13441,7 @@
         <v>0.50346809625625599</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-9606</v>
       </c>
@@ -13463,7 +13478,7 @@
       </c>
       <c r="N9">
         <f t="shared" si="3"/>
-        <v>-5550.1272727272735</v>
+        <v>-5804.6727272727276</v>
       </c>
       <c r="O9">
         <f t="shared" si="3"/>
@@ -13493,7 +13508,7 @@
         <v>3178</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-9916</v>
       </c>
@@ -13530,7 +13545,7 @@
       </c>
       <c r="N10">
         <f t="shared" si="3"/>
-        <v>-5805.9454545454555</v>
+        <v>-6096.8545454545465</v>
       </c>
       <c r="O10">
         <f t="shared" si="3"/>
@@ -13553,14 +13568,14 @@
       </c>
       <c r="U10">
         <f>(U4-U6-U9)/(U7-1)</f>
-        <v>-74.218181818181819</v>
+        <v>-110.58181818181818</v>
       </c>
       <c r="V10">
         <f>(V4-V6-V9)/(V7-1)</f>
         <v>2.0909090909090908</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-9916</v>
       </c>
@@ -13597,7 +13612,7 @@
       </c>
       <c r="N11">
         <f t="shared" si="3"/>
-        <v>-5996.363636363636</v>
+        <v>-6323.6363636363631</v>
       </c>
       <c r="O11">
         <f t="shared" si="3"/>
@@ -13616,7 +13631,7 @@
         <v>0.50346809625625599</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-10187</v>
       </c>
@@ -13653,7 +13668,7 @@
       </c>
       <c r="N12">
         <f t="shared" si="3"/>
-        <v>-6237.9818181818173</v>
+        <v>-6601.6181818181813</v>
       </c>
       <c r="O12">
         <f t="shared" si="3"/>
@@ -13672,7 +13687,7 @@
         <v>0.50346809625625599</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-10187</v>
       </c>
@@ -13709,7 +13724,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="3"/>
-        <v>-6417.6</v>
+        <v>-6817.6</v>
       </c>
       <c r="O13">
         <f t="shared" si="3"/>
@@ -13728,7 +13743,7 @@
         <v>0.50346809625625599</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-10443</v>
       </c>
@@ -13765,7 +13780,7 @@
       </c>
       <c r="N14">
         <f t="shared" si="3"/>
-        <v>-6651.2181818181825</v>
+        <v>-7087.5818181818186</v>
       </c>
       <c r="O14">
         <f t="shared" si="3"/>
@@ -13784,7 +13799,7 @@
         <v>0.50346809625625599</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-10443</v>
       </c>
@@ -13821,7 +13836,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="3"/>
-        <v>-6830.6363636363631</v>
+        <v>-7303.363636363636</v>
       </c>
       <c r="O15">
         <f t="shared" si="3"/>
@@ -13840,7 +13855,7 @@
         <v>0.50346809625625599</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-10713</v>
       </c>
@@ -13877,7 +13892,7 @@
       </c>
       <c r="N16">
         <f t="shared" si="3"/>
-        <v>-7059.8545454545447</v>
+        <v>-7568.9454545454537</v>
       </c>
       <c r="O16">
         <f t="shared" si="3"/>
@@ -13933,7 +13948,7 @@
       </c>
       <c r="N17">
         <f t="shared" si="3"/>
-        <v>-7237.8727272727274</v>
+        <v>-7783.3272727272733</v>
       </c>
       <c r="O17">
         <f t="shared" si="3"/>
@@ -13989,7 +14004,7 @@
       </c>
       <c r="N18">
         <f t="shared" si="3"/>
-        <v>-7454.6909090909103</v>
+        <v>-8036.5090909090914</v>
       </c>
       <c r="O18">
         <f t="shared" si="3"/>
@@ -14045,7 +14060,7 @@
       </c>
       <c r="N19">
         <f t="shared" ref="N19:O34" si="7">H19+U$9 +($M18*U$10)</f>
-        <v>-7617.5090909090904</v>
+        <v>-8235.6909090909085</v>
       </c>
       <c r="O19">
         <f t="shared" si="7"/>
@@ -14101,7 +14116,7 @@
       </c>
       <c r="N20">
         <f t="shared" si="7"/>
-        <v>-7808.3272727272724</v>
+        <v>-8462.8727272727265</v>
       </c>
       <c r="O20">
         <f t="shared" si="7"/>
@@ -14157,7 +14172,7 @@
       </c>
       <c r="N21">
         <f t="shared" si="7"/>
-        <v>-7949.3454545454551</v>
+        <v>-8640.254545454547</v>
       </c>
       <c r="O21">
         <f t="shared" si="7"/>
@@ -14213,7 +14228,7 @@
       </c>
       <c r="N22">
         <f t="shared" si="7"/>
-        <v>-8108.9636363636364</v>
+        <v>-8836.2363636363643</v>
       </c>
       <c r="O22">
         <f t="shared" si="7"/>
@@ -14269,7 +14284,7 @@
       </c>
       <c r="N23">
         <f t="shared" si="7"/>
-        <v>-8229.7818181818184</v>
+        <v>-8993.4181818181823</v>
       </c>
       <c r="O23">
         <f t="shared" si="7"/>
@@ -14325,7 +14340,7 @@
       </c>
       <c r="N24">
         <f t="shared" si="7"/>
-        <v>-8363</v>
+        <v>-9163</v>
       </c>
       <c r="O24">
         <f t="shared" si="7"/>
@@ -14381,7 +14396,7 @@
       </c>
       <c r="N25">
         <f t="shared" si="7"/>
-        <v>-8468.2181818181816</v>
+        <v>-9304.5818181818195</v>
       </c>
       <c r="O25">
         <f t="shared" si="7"/>
@@ -14437,7 +14452,7 @@
       </c>
       <c r="N26">
         <f t="shared" si="7"/>
-        <v>-8572.8363636363647</v>
+        <v>-9445.5636363636368</v>
       </c>
       <c r="O26">
         <f t="shared" si="7"/>
@@ -14493,7 +14508,7 @@
       </c>
       <c r="N27">
         <f t="shared" si="7"/>
-        <v>-8658.8545454545456</v>
+        <v>-9567.9454545454537</v>
       </c>
       <c r="O27">
         <f t="shared" si="7"/>
@@ -14549,7 +14564,7 @@
       </c>
       <c r="N28">
         <f t="shared" si="7"/>
-        <v>-8739.4727272727268</v>
+        <v>-9684.9272727272728</v>
       </c>
       <c r="O28">
         <f t="shared" si="7"/>
@@ -14605,7 +14620,7 @@
       </c>
       <c r="N29">
         <f t="shared" si="7"/>
-        <v>-8807.6909090909085</v>
+        <v>-9789.5090909090904</v>
       </c>
       <c r="O29">
         <f t="shared" si="7"/>
@@ -14661,7 +14676,7 @@
       </c>
       <c r="N30">
         <f t="shared" si="7"/>
-        <v>-8872.1090909090908</v>
+        <v>-9890.2909090909088</v>
       </c>
       <c r="O30">
         <f t="shared" si="7"/>
@@ -14717,7 +14732,7 @@
       </c>
       <c r="N31">
         <f t="shared" si="7"/>
-        <v>-8937.1272727272717</v>
+        <v>-9991.6727272727258</v>
       </c>
       <c r="O31">
         <f t="shared" si="7"/>
@@ -14773,7 +14788,7 @@
       </c>
       <c r="N32">
         <f t="shared" si="7"/>
-        <v>-9004.9454545454537</v>
+        <v>-10095.854545454546</v>
       </c>
       <c r="O32">
         <f t="shared" si="7"/>
@@ -14829,7 +14844,7 @@
       </c>
       <c r="N33">
         <f t="shared" si="7"/>
-        <v>-9078.1636363636353</v>
+        <v>-10205.436363636363</v>
       </c>
       <c r="O33">
         <f t="shared" si="7"/>
@@ -14885,7 +14900,7 @@
       </c>
       <c r="N34">
         <f t="shared" si="7"/>
-        <v>-9151.3818181818169</v>
+        <v>-10315.018181818181</v>
       </c>
       <c r="O34">
         <f t="shared" si="7"/>
@@ -14941,7 +14956,7 @@
       </c>
       <c r="N35">
         <f t="shared" ref="N35:O50" si="9">H35+U$9 +($M34*U$10)</f>
-        <v>-9228.4000000000015</v>
+        <v>-10428.400000000001</v>
       </c>
       <c r="O35">
         <f t="shared" si="9"/>
@@ -14997,7 +15012,7 @@
       </c>
       <c r="N36">
         <f t="shared" si="9"/>
-        <v>-9305.4181818181823</v>
+        <v>-10541.781818181818</v>
       </c>
       <c r="O36">
         <f t="shared" si="9"/>
@@ -15053,7 +15068,7 @@
       </c>
       <c r="N37">
         <f t="shared" si="9"/>
-        <v>-9379.4363636363632</v>
+        <v>-10652.163636363635</v>
       </c>
       <c r="O37">
         <f t="shared" si="9"/>
@@ -15109,7 +15124,7 @@
       </c>
       <c r="N38">
         <f t="shared" si="9"/>
-        <v>-9453.454545454546</v>
+        <v>-10762.545454545456</v>
       </c>
       <c r="O38">
         <f t="shared" si="9"/>
@@ -15165,7 +15180,7 @@
       </c>
       <c r="N39">
         <f t="shared" si="9"/>
-        <v>-9527.4727272727268</v>
+        <v>-10872.927272727273</v>
       </c>
       <c r="O39">
         <f t="shared" si="9"/>
@@ -15221,7 +15236,7 @@
       </c>
       <c r="N40">
         <f t="shared" si="9"/>
-        <v>-9601.4909090909096</v>
+        <v>-10983.309090909092</v>
       </c>
       <c r="O40">
         <f t="shared" si="9"/>
@@ -15277,7 +15292,7 @@
       </c>
       <c r="N41">
         <f t="shared" si="9"/>
-        <v>-9678.7090909090912</v>
+        <v>-11096.890909090911</v>
       </c>
       <c r="O41">
         <f t="shared" si="9"/>
@@ -15333,7 +15348,7 @@
       </c>
       <c r="N42">
         <f t="shared" si="9"/>
-        <v>-9756.1272727272735</v>
+        <v>-11210.672727272726</v>
       </c>
       <c r="O42">
         <f t="shared" si="9"/>
@@ -15389,7 +15404,7 @@
       </c>
       <c r="N43">
         <f t="shared" si="9"/>
-        <v>-9870.745454545453</v>
+        <v>-11361.654545454545</v>
       </c>
       <c r="O43">
         <f t="shared" si="9"/>
@@ -15445,7 +15460,7 @@
       </c>
       <c r="N44">
         <f t="shared" si="9"/>
-        <v>-9985.363636363636</v>
+        <v>-11512.636363636364</v>
       </c>
       <c r="O44">
         <f t="shared" si="9"/>
@@ -15501,7 +15516,7 @@
       </c>
       <c r="N45">
         <f t="shared" si="9"/>
-        <v>-10221.581818181819</v>
+        <v>-11785.218181818182</v>
       </c>
       <c r="O45">
         <f t="shared" si="9"/>
@@ -15557,7 +15572,7 @@
       </c>
       <c r="N46">
         <f t="shared" si="9"/>
-        <v>-10454.6</v>
+        <v>-12054.599999999999</v>
       </c>
       <c r="O46">
         <f t="shared" si="9"/>
@@ -15613,7 +15628,7 @@
       </c>
       <c r="N47">
         <f t="shared" si="9"/>
-        <v>-10875.418181818182</v>
+        <v>-12511.781818181818</v>
       </c>
       <c r="O47">
         <f t="shared" si="9"/>
@@ -15669,7 +15684,7 @@
       </c>
       <c r="N48">
         <f t="shared" si="9"/>
-        <v>-11486.636363636364</v>
+        <v>-13159.363636363636</v>
       </c>
       <c r="O48">
         <f t="shared" si="9"/>
@@ -15725,7 +15740,7 @@
       </c>
       <c r="N49">
         <f t="shared" si="9"/>
-        <v>-12097.854545454546</v>
+        <v>-13806.945454545454</v>
       </c>
       <c r="O49">
         <f t="shared" si="9"/>
@@ -15781,7 +15796,7 @@
       </c>
       <c r="N50">
         <f t="shared" si="9"/>
-        <v>-12587.472727272727</v>
+        <v>-14332.927272727273</v>
       </c>
       <c r="O50">
         <f t="shared" si="9"/>
@@ -15837,7 +15852,7 @@
       </c>
       <c r="N51">
         <f t="shared" ref="N51:O66" si="11">H51+U$9 +($M50*U$10)</f>
-        <v>-13077.090909090908</v>
+        <v>-14858.90909090909</v>
       </c>
       <c r="O51">
         <f t="shared" si="11"/>
@@ -15893,7 +15908,7 @@
       </c>
       <c r="N52">
         <f t="shared" si="11"/>
-        <v>-13621.909090909092</v>
+        <v>-15440.090909090908</v>
       </c>
       <c r="O52">
         <f t="shared" si="11"/>
@@ -15949,7 +15964,7 @@
       </c>
       <c r="N53">
         <f t="shared" si="11"/>
-        <v>-13939.127272727274</v>
+        <v>-15793.672727272726</v>
       </c>
       <c r="O53">
         <f t="shared" si="11"/>
@@ -16005,7 +16020,7 @@
       </c>
       <c r="N54">
         <f t="shared" si="11"/>
-        <v>-14486.745454545455</v>
+        <v>-16377.654545454545</v>
       </c>
       <c r="O54">
         <f t="shared" si="11"/>
@@ -16061,7 +16076,7 @@
       </c>
       <c r="N55">
         <f t="shared" si="11"/>
-        <v>-15034.363636363636</v>
+        <v>-16961.636363636364</v>
       </c>
       <c r="O55">
         <f t="shared" si="11"/>
@@ -16117,7 +16132,7 @@
       </c>
       <c r="N56">
         <f t="shared" si="11"/>
-        <v>-15804.981818181819</v>
+        <v>-17768.618181818183</v>
       </c>
       <c r="O56">
         <f t="shared" si="11"/>
@@ -16173,7 +16188,7 @@
       </c>
       <c r="N57">
         <f t="shared" si="11"/>
-        <v>-16332.599999999999</v>
+        <v>-18332.599999999999</v>
       </c>
       <c r="O57">
         <f t="shared" si="11"/>
@@ -16229,7 +16244,7 @@
       </c>
       <c r="N58">
         <f t="shared" si="11"/>
-        <v>-17093.81818181818</v>
+        <v>-19130.181818181816</v>
       </c>
       <c r="O58">
         <f t="shared" si="11"/>
@@ -16285,7 +16300,7 @@
       </c>
       <c r="N59">
         <f t="shared" si="11"/>
-        <v>-17624.636363636364</v>
+        <v>-19697.363636363636</v>
       </c>
       <c r="O59">
         <f t="shared" si="11"/>
@@ -16341,7 +16356,7 @@
       </c>
       <c r="N60">
         <f t="shared" si="11"/>
-        <v>-18392.854545454546</v>
+        <v>-20501.945454545457</v>
       </c>
       <c r="O60">
         <f t="shared" si="11"/>
@@ -16397,7 +16412,7 @@
       </c>
       <c r="N61">
         <f t="shared" si="11"/>
-        <v>-18938.072727272727</v>
+        <v>-21083.527272727275</v>
       </c>
       <c r="O61">
         <f t="shared" si="11"/>
@@ -16453,7 +16468,7 @@
       </c>
       <c r="N62">
         <f t="shared" si="11"/>
-        <v>-19712.890909090907</v>
+        <v>-21894.709090909091</v>
       </c>
       <c r="O62">
         <f t="shared" si="11"/>
@@ -16509,7 +16524,7 @@
       </c>
       <c r="N63">
         <f t="shared" si="11"/>
-        <v>-20254.109090909089</v>
+        <v>-22472.290909090909</v>
       </c>
       <c r="O63">
         <f t="shared" si="11"/>
@@ -16565,7 +16580,7 @@
       </c>
       <c r="N64">
         <f t="shared" si="11"/>
-        <v>-21019.527272727275</v>
+        <v>-23274.072727272727</v>
       </c>
       <c r="O64">
         <f t="shared" si="11"/>
@@ -16621,7 +16636,7 @@
       </c>
       <c r="N65">
         <f t="shared" si="11"/>
-        <v>-21547.545454545456</v>
+        <v>-23838.454545454544</v>
       </c>
       <c r="O65">
         <f t="shared" si="11"/>
@@ -16677,7 +16692,7 @@
       </c>
       <c r="N66">
         <f t="shared" si="11"/>
-        <v>-22304.563636363637</v>
+        <v>-24631.836363636361</v>
       </c>
       <c r="O66">
         <f t="shared" si="11"/>
@@ -16692,7 +16707,7 @@
         <v>-5470.2</v>
       </c>
       <c r="R66">
-        <f t="shared" ref="R66:R111" si="13">E66</f>
+        <f t="shared" ref="R66:R109" si="13">E66</f>
         <v>0.44008195400237998</v>
       </c>
     </row>
@@ -16733,14 +16748,14 @@
       </c>
       <c r="N67">
         <f t="shared" ref="N67:O82" si="14">H67+U$9 +($M66*U$10)</f>
-        <v>-22831.981818181819</v>
+        <v>-25195.618181818179</v>
       </c>
       <c r="O67">
         <f t="shared" si="14"/>
         <v>-43548.69090909091</v>
       </c>
       <c r="P67">
-        <f t="shared" ref="P67:Q108" si="15">J67</f>
+        <f t="shared" ref="P67:Q106" si="15">J67</f>
         <v>-5758.2</v>
       </c>
       <c r="Q67">
@@ -16789,7 +16804,7 @@
       </c>
       <c r="N68">
         <f t="shared" si="14"/>
-        <v>-23589</v>
+        <v>-25989</v>
       </c>
       <c r="O68">
         <f t="shared" si="14"/>
@@ -16845,7 +16860,7 @@
       </c>
       <c r="N69">
         <f t="shared" si="14"/>
-        <v>-24121.818181818184</v>
+        <v>-26558.18181818182</v>
       </c>
       <c r="O69">
         <f t="shared" si="14"/>
@@ -16901,7 +16916,7 @@
       </c>
       <c r="N70">
         <f t="shared" si="14"/>
-        <v>-24875.036363636365</v>
+        <v>-27347.763636363637</v>
       </c>
       <c r="O70">
         <f t="shared" si="14"/>
@@ -16957,7 +16972,7 @@
       </c>
       <c r="N71">
         <f t="shared" si="14"/>
-        <v>-25399.254545454547</v>
+        <v>-27908.345454545455</v>
       </c>
       <c r="O71">
         <f t="shared" si="14"/>
@@ -17013,7 +17028,7 @@
       </c>
       <c r="N72">
         <f t="shared" si="14"/>
-        <v>-26132.872727272726</v>
+        <v>-28678.327272727271</v>
       </c>
       <c r="O72">
         <f t="shared" si="14"/>
@@ -17069,7 +17084,7 @@
       </c>
       <c r="N73">
         <f t="shared" si="14"/>
-        <v>-26636.890909090911</v>
+        <v>-29218.709090909091</v>
       </c>
       <c r="O73">
         <f t="shared" si="14"/>
@@ -17125,7 +17140,7 @@
       </c>
       <c r="N74">
         <f t="shared" si="14"/>
-        <v>-27348.909090909092</v>
+        <v>-29967.090909090912</v>
       </c>
       <c r="O74">
         <f t="shared" si="14"/>
@@ -17181,7 +17196,7 @@
       </c>
       <c r="N75">
         <f t="shared" si="14"/>
-        <v>-27840.527272727271</v>
+        <v>-30495.072727272724</v>
       </c>
       <c r="O75">
         <f t="shared" si="14"/>
@@ -17237,7 +17252,7 @@
       </c>
       <c r="N76">
         <f t="shared" si="14"/>
-        <v>-28541.945454545454</v>
+        <v>-31232.854545454546</v>
       </c>
       <c r="O76">
         <f t="shared" si="14"/>
@@ -17293,7 +17308,7 @@
       </c>
       <c r="N77">
         <f t="shared" si="14"/>
-        <v>-29033.963636363635</v>
+        <v>-31761.236363636363</v>
       </c>
       <c r="O77">
         <f t="shared" si="14"/>
@@ -17349,7 +17364,7 @@
       </c>
       <c r="N78">
         <f t="shared" si="14"/>
-        <v>-29736.181818181816</v>
+        <v>-32499.81818181818</v>
       </c>
       <c r="O78">
         <f t="shared" si="14"/>
@@ -17405,7 +17420,7 @@
       </c>
       <c r="N79">
         <f t="shared" si="14"/>
-        <v>-30230.399999999998</v>
+        <v>-33030.399999999994</v>
       </c>
       <c r="O79">
         <f t="shared" si="14"/>
@@ -17461,7 +17476,7 @@
       </c>
       <c r="N80">
         <f t="shared" si="14"/>
-        <v>-30934.018181818181</v>
+        <v>-33770.381818181821</v>
       </c>
       <c r="O80">
         <f t="shared" si="14"/>
@@ -17517,7 +17532,7 @@
       </c>
       <c r="N81">
         <f t="shared" si="14"/>
-        <v>-31427.836363636361</v>
+        <v>-34300.563636363637</v>
       </c>
       <c r="O81">
         <f t="shared" si="14"/>
@@ -17573,7 +17588,7 @@
       </c>
       <c r="N82">
         <f t="shared" si="14"/>
-        <v>-32121.854545454546</v>
+        <v>-35030.945454545457</v>
       </c>
       <c r="O82">
         <f t="shared" si="14"/>
@@ -17629,7 +17644,7 @@
       </c>
       <c r="N83">
         <f t="shared" ref="N83:O98" si="17">H83+U$9 +($M82*U$10)</f>
-        <v>-32605.672727272729</v>
+        <v>-35551.127272727274</v>
       </c>
       <c r="O83">
         <f t="shared" si="17"/>
@@ -17685,7 +17700,7 @@
       </c>
       <c r="N84">
         <f t="shared" si="17"/>
-        <v>-33089.490909090906</v>
+        <v>-36071.30909090909</v>
       </c>
       <c r="O84">
         <f t="shared" si="17"/>
@@ -17741,7 +17756,7 @@
       </c>
       <c r="N85">
         <f t="shared" si="17"/>
-        <v>-33732.109090909093</v>
+        <v>-36750.290909090909</v>
       </c>
       <c r="O85">
         <f t="shared" si="17"/>
@@ -17797,7 +17812,7 @@
       </c>
       <c r="N86">
         <f t="shared" si="17"/>
-        <v>-34374.727272727272</v>
+        <v>-37429.272727272728</v>
       </c>
       <c r="O86">
         <f t="shared" si="17"/>
@@ -17853,7 +17868,7 @@
       </c>
       <c r="N87">
         <f t="shared" si="17"/>
-        <v>-34983.945454545457</v>
+        <v>-38074.854545454546</v>
       </c>
       <c r="O87">
         <f t="shared" si="17"/>
@@ -17909,7 +17924,7 @@
       </c>
       <c r="N88">
         <f t="shared" si="17"/>
-        <v>-35593.163636363635</v>
+        <v>-38720.436363636363</v>
       </c>
       <c r="O88">
         <f t="shared" si="17"/>
@@ -17965,7 +17980,7 @@
       </c>
       <c r="N89">
         <f t="shared" si="17"/>
-        <v>-36357.581818181818</v>
+        <v>-39521.218181818178</v>
       </c>
       <c r="O89">
         <f t="shared" si="17"/>
@@ -18021,7 +18036,7 @@
       </c>
       <c r="N90">
         <f t="shared" si="17"/>
-        <v>-36753.799999999996</v>
+        <v>-39953.799999999996</v>
       </c>
       <c r="O90">
         <f t="shared" si="17"/>
@@ -18077,7 +18092,7 @@
       </c>
       <c r="N91">
         <f t="shared" si="17"/>
-        <v>-37298.018181818181</v>
+        <v>-40534.381818181821</v>
       </c>
       <c r="O91">
         <f t="shared" si="17"/>
@@ -18133,7 +18148,7 @@
       </c>
       <c r="N92">
         <f t="shared" si="17"/>
-        <v>-37675.436363636371</v>
+        <v>-40948.163636363635</v>
       </c>
       <c r="O92">
         <f t="shared" si="17"/>
@@ -18189,7 +18204,7 @@
       </c>
       <c r="N93">
         <f t="shared" si="17"/>
-        <v>-38052.854545454546</v>
+        <v>-41361.94545454545</v>
       </c>
       <c r="O93">
         <f t="shared" si="17"/>
@@ -18245,7 +18260,7 @@
       </c>
       <c r="N94">
         <f t="shared" si="17"/>
-        <v>-38422.472727272732</v>
+        <v>-41767.927272727276</v>
       </c>
       <c r="O94">
         <f t="shared" si="17"/>
@@ -18301,7 +18316,7 @@
       </c>
       <c r="N95">
         <f t="shared" si="17"/>
-        <v>-38792.090909090912</v>
+        <v>-42173.909090909096</v>
       </c>
       <c r="O95">
         <f t="shared" si="17"/>
@@ -18357,7 +18372,7 @@
       </c>
       <c r="N96">
         <f t="shared" si="17"/>
-        <v>-39154.909090909096</v>
+        <v>-42573.090909090912</v>
       </c>
       <c r="O96">
         <f t="shared" si="17"/>
@@ -18413,7 +18428,7 @@
       </c>
       <c r="N97">
         <f t="shared" si="17"/>
-        <v>-39517.727272727272</v>
+        <v>-42972.272727272728</v>
       </c>
       <c r="O97">
         <f t="shared" si="17"/>
@@ -18469,7 +18484,7 @@
       </c>
       <c r="N98">
         <f t="shared" si="17"/>
-        <v>-40012.145454545454</v>
+        <v>-43503.054545454543</v>
       </c>
       <c r="O98">
         <f t="shared" si="17"/>
@@ -18524,8 +18539,8 @@
         <v>98</v>
       </c>
       <c r="N99">
-        <f t="shared" ref="N99:O108" si="19">H99+U$9 +($M98*U$10)</f>
-        <v>-40359.163636363635</v>
+        <f t="shared" ref="N99:O106" si="19">H99+U$9 +($M98*U$10)</f>
+        <v>-43886.436363636363</v>
       </c>
       <c r="O99">
         <f t="shared" si="19"/>
@@ -18581,7 +18596,7 @@
       </c>
       <c r="N100">
         <f t="shared" si="19"/>
-        <v>-40833.781818181822</v>
+        <v>-44397.418181818182</v>
       </c>
       <c r="O100">
         <f t="shared" si="19"/>
@@ -18637,7 +18652,7 @@
       </c>
       <c r="N101">
         <f t="shared" si="19"/>
-        <v>-41167.199999999997</v>
+        <v>-44767.199999999997</v>
       </c>
       <c r="O101">
         <f t="shared" si="19"/>
@@ -18693,7 +18708,7 @@
       </c>
       <c r="N102">
         <f t="shared" si="19"/>
-        <v>-41629.218181818185</v>
+        <v>-45265.581818181818</v>
       </c>
       <c r="O102">
         <f t="shared" si="19"/>
@@ -18749,7 +18764,7 @@
       </c>
       <c r="N103">
         <f t="shared" si="19"/>
-        <v>-41959.63636363636</v>
+        <v>-45632.363636363632</v>
       </c>
       <c r="O103">
         <f t="shared" si="19"/>
@@ -18805,7 +18820,7 @@
       </c>
       <c r="N104">
         <f t="shared" si="19"/>
-        <v>-42421.05454545455</v>
+        <v>-46130.145454545454</v>
       </c>
       <c r="O104">
         <f t="shared" si="19"/>
@@ -18861,7 +18876,7 @@
       </c>
       <c r="N105">
         <f>H105+U$9 +($M104*U$10)</f>
-        <v>-42754.872727272726</v>
+        <v>-46500.327272727271</v>
       </c>
       <c r="O105">
         <f t="shared" si="19"/>
@@ -18917,7 +18932,7 @@
       </c>
       <c r="N106">
         <f>H106+U$9 +($M105*U$10)</f>
-        <v>-43214.890909090907</v>
+        <v>-46996.709090909091</v>
       </c>
       <c r="O106">
         <f t="shared" si="19"/>
@@ -18973,7 +18988,7 @@
       </c>
       <c r="N107">
         <f t="shared" ref="N107:N112" si="21">H107+U$9 +($M106*U$10)</f>
-        <v>-43546.30909090909</v>
+        <v>-47364.490909090906</v>
       </c>
       <c r="O107">
         <f t="shared" ref="O107:O112" si="22">I107+V$9 +($M106*V$10)</f>
@@ -19029,7 +19044,7 @@
       </c>
       <c r="N108">
         <f t="shared" si="21"/>
-        <v>-43992.327272727271</v>
+        <v>-47846.872727272726</v>
       </c>
       <c r="O108">
         <f t="shared" si="22"/>
@@ -19085,7 +19100,7 @@
       </c>
       <c r="N109">
         <f t="shared" si="21"/>
-        <v>-44307.345454545452</v>
+        <v>-48198.254545454547</v>
       </c>
       <c r="O109">
         <f t="shared" si="22"/>
@@ -19141,7 +19156,7 @@
       </c>
       <c r="N110">
         <f t="shared" si="21"/>
-        <v>-44381.563636363637</v>
+        <v>-48308.836363636365</v>
       </c>
       <c r="O110">
         <f t="shared" si="22"/>
@@ -19185,7 +19200,7 @@
         <v>-53398.666666666664</v>
       </c>
       <c r="J111">
-        <f t="shared" ref="I111:K111" si="30">AVERAGE(C109:C111)</f>
+        <f t="shared" ref="J111:K111" si="30">AVERAGE(C109:C111)</f>
         <v>-3169.6666666666665</v>
       </c>
       <c r="K111">
@@ -19197,7 +19212,7 @@
       </c>
       <c r="N111">
         <f t="shared" si="21"/>
-        <v>-44734.781818181815</v>
+        <v>-48698.418181818182</v>
       </c>
       <c r="O111">
         <f t="shared" si="22"/>
@@ -19253,7 +19268,7 @@
       </c>
       <c r="N112">
         <f t="shared" si="21"/>
-        <v>-45000</v>
+        <v>-49000</v>
       </c>
       <c r="O112">
         <f t="shared" si="22"/>
@@ -31321,7 +31336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4452A2C0-D173-4635-89B3-218927C8FDC6}">
   <dimension ref="A1:V268"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N1" sqref="N1:R1048576"/>
     </sheetView>
   </sheetViews>
@@ -42378,7 +42393,7 @@
         <v>0.23206001500000001</v>
       </c>
       <c r="H101">
-        <f t="shared" ref="H101:K109" si="20">AVERAGE(A99:A103)</f>
+        <f t="shared" ref="H101:K102" si="20">AVERAGE(A99:A103)</f>
         <v>-59550.400000000001</v>
       </c>
       <c r="I101">
@@ -42490,19 +42505,19 @@
         <v>0.23206001500000001</v>
       </c>
       <c r="H103">
-        <f t="shared" ref="H103:H144" si="21">AVERAGE(A101:A105)</f>
+        <f t="shared" ref="H103:H142" si="21">AVERAGE(A101:A105)</f>
         <v>-59137.8</v>
       </c>
       <c r="I103">
-        <f t="shared" ref="I103:I144" si="22">AVERAGE(B101:B105)</f>
+        <f t="shared" ref="I103:I142" si="22">AVERAGE(B101:B105)</f>
         <v>66322</v>
       </c>
       <c r="J103">
-        <f t="shared" ref="J103:J144" si="23">AVERAGE(C101:C105)</f>
+        <f t="shared" ref="J103:J142" si="23">AVERAGE(C101:C105)</f>
         <v>1018.8</v>
       </c>
       <c r="K103">
-        <f t="shared" ref="K103:K144" si="24">AVERAGE(D101:D105)</f>
+        <f t="shared" ref="K103:K142" si="24">AVERAGE(D101:D105)</f>
         <v>3879</v>
       </c>
       <c r="M103">

</xml_diff>

<commit_message>
Competition path adjustments, added ability to change operator level selection while running path, fixed distal arm adj bug
</commit_message>
<xml_diff>
--- a/ROBOT_CODE/AlexanderGCowbell/src/main/java/frc/data/mp/SmoothedPaths.xlsx
+++ b/ROBOT_CODE/AlexanderGCowbell/src/main/java/frc/data/mp/SmoothedPaths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SHARED\FRC2023\ROBOT_CODE\AlexanderGCowbell\src\main\java\frc\data\mp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF03287-1CF0-483F-9314-5E29A808B84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C89064-61DC-4AC5-854D-725367692560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thief1" sheetId="16" r:id="rId1"/>
@@ -5136,8 +5136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B7D99D-F1DF-47C3-91B6-FDAE4C5C3FE7}">
   <dimension ref="A1:V340"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:R1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5298,7 +5298,7 @@
       </c>
       <c r="O3">
         <f t="shared" si="3"/>
-        <v>10398.720657276996</v>
+        <v>10391.171361502347</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:Q66" si="4">J3</f>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="O4">
         <f t="shared" si="3"/>
-        <v>10542.974647887324</v>
+        <v>10527.876056338029</v>
       </c>
       <c r="P4">
         <f t="shared" si="4"/>
@@ -5384,7 +5384,7 @@
         <v>-35000</v>
       </c>
       <c r="V4" s="3">
-        <v>68000</v>
+        <v>66928</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -5428,7 +5428,7 @@
       </c>
       <c r="O5">
         <f t="shared" si="3"/>
-        <v>10669.961971830986</v>
+        <v>10647.314084507041</v>
       </c>
       <c r="P5">
         <f t="shared" si="4"/>
@@ -5495,7 +5495,7 @@
       </c>
       <c r="O6">
         <f t="shared" si="3"/>
-        <v>10878.149295774649</v>
+        <v>10847.952112676057</v>
       </c>
       <c r="P6">
         <f t="shared" si="4"/>
@@ -5562,7 +5562,7 @@
       </c>
       <c r="O7">
         <f t="shared" si="3"/>
-        <v>11034.53661971831</v>
+        <v>10996.790140845071</v>
       </c>
       <c r="P7">
         <f t="shared" si="4"/>
@@ -5629,7 +5629,7 @@
       </c>
       <c r="O8">
         <f t="shared" si="3"/>
-        <v>11286.923943661972</v>
+        <v>11241.628169014084</v>
       </c>
       <c r="P8">
         <f t="shared" si="4"/>
@@ -5685,7 +5685,7 @@
       </c>
       <c r="O9">
         <f t="shared" si="3"/>
-        <v>11476.511267605632</v>
+        <v>11423.666197183098</v>
       </c>
       <c r="P9">
         <f t="shared" si="4"/>
@@ -5752,7 +5752,7 @@
       </c>
       <c r="O10">
         <f t="shared" si="3"/>
-        <v>11771.298591549297</v>
+        <v>11710.904225352113</v>
       </c>
       <c r="P10">
         <f t="shared" si="4"/>
@@ -5775,7 +5775,7 @@
       </c>
       <c r="V10">
         <f>(V4-V6-V9)/(V7-1)</f>
-        <v>12.387323943661972</v>
+        <v>4.8380281690140849</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -5819,7 +5819,7 @@
       </c>
       <c r="O11">
         <f t="shared" si="3"/>
-        <v>11984.885915492958</v>
+        <v>11916.942253521127</v>
       </c>
       <c r="P11">
         <f t="shared" si="4"/>
@@ -5875,7 +5875,7 @@
       </c>
       <c r="O12">
         <f t="shared" si="3"/>
-        <v>12428.07323943662</v>
+        <v>12352.580281690141</v>
       </c>
       <c r="P12">
         <f t="shared" si="4"/>
@@ -5931,7 +5931,7 @@
       </c>
       <c r="O13">
         <f t="shared" si="3"/>
-        <v>12775.260563380281</v>
+        <v>12692.218309859154</v>
       </c>
       <c r="P13">
         <f t="shared" si="4"/>
@@ -5987,7 +5987,7 @@
       </c>
       <c r="O14">
         <f t="shared" si="3"/>
-        <v>13122.447887323942</v>
+        <v>13031.856338028168</v>
       </c>
       <c r="P14">
         <f t="shared" si="4"/>
@@ -6043,7 +6043,7 @@
       </c>
       <c r="O15">
         <f t="shared" si="3"/>
-        <v>13493.435211267606</v>
+        <v>13395.294366197182</v>
       </c>
       <c r="P15">
         <f t="shared" si="4"/>
@@ -6099,7 +6099,7 @@
       </c>
       <c r="O16">
         <f t="shared" si="3"/>
-        <v>13864.422535211268</v>
+        <v>13758.732394366198</v>
       </c>
       <c r="P16">
         <f t="shared" si="4"/>
@@ -6155,7 +6155,7 @@
       </c>
       <c r="O17">
         <f t="shared" si="3"/>
-        <v>14146.209859154929</v>
+        <v>14032.970422535211</v>
       </c>
       <c r="P17">
         <f t="shared" si="4"/>
@@ -6211,7 +6211,7 @@
       </c>
       <c r="O18">
         <f t="shared" si="3"/>
-        <v>14427.997183098591</v>
+        <v>14307.208450704225</v>
       </c>
       <c r="P18">
         <f t="shared" si="4"/>
@@ -6267,7 +6267,7 @@
       </c>
       <c r="O19">
         <f t="shared" si="7"/>
-        <v>14859.784507042254</v>
+        <v>14731.44647887324</v>
       </c>
       <c r="P19">
         <f t="shared" si="4"/>
@@ -6323,7 +6323,7 @@
       </c>
       <c r="O20">
         <f t="shared" si="7"/>
-        <v>15162.571830985915</v>
+        <v>15026.684507042251</v>
       </c>
       <c r="P20">
         <f t="shared" si="4"/>
@@ -6379,7 +6379,7 @@
       </c>
       <c r="O21">
         <f t="shared" si="7"/>
-        <v>15628.159154929577</v>
+        <v>15484.722535211267</v>
       </c>
       <c r="P21">
         <f t="shared" si="4"/>
@@ -6435,7 +6435,7 @@
       </c>
       <c r="O22">
         <f t="shared" si="7"/>
-        <v>15953.346478873238</v>
+        <v>15802.36056338028</v>
       </c>
       <c r="P22">
         <f t="shared" si="4"/>
@@ -6491,7 +6491,7 @@
       </c>
       <c r="O23">
         <f t="shared" si="7"/>
-        <v>16278.533802816903</v>
+        <v>16119.998591549298</v>
       </c>
       <c r="P23">
         <f t="shared" si="4"/>
@@ -6547,7 +6547,7 @@
       </c>
       <c r="O24">
         <f t="shared" si="7"/>
-        <v>16626.321126760562</v>
+        <v>16460.236619718307</v>
       </c>
       <c r="P24">
         <f t="shared" si="4"/>
@@ -6603,7 +6603,7 @@
       </c>
       <c r="O25">
         <f t="shared" si="7"/>
-        <v>16974.108450704225</v>
+        <v>16800.474647887324</v>
       </c>
       <c r="P25">
         <f t="shared" si="4"/>
@@ -6659,7 +6659,7 @@
       </c>
       <c r="O26">
         <f t="shared" si="7"/>
-        <v>17336.295774647886</v>
+        <v>17155.112676056338</v>
       </c>
       <c r="P26">
         <f t="shared" si="4"/>
@@ -6715,7 +6715,7 @@
       </c>
       <c r="O27">
         <f t="shared" si="7"/>
-        <v>17698.483098591547</v>
+        <v>17509.750704225353</v>
       </c>
       <c r="P27">
         <f t="shared" si="4"/>
@@ -6771,7 +6771,7 @@
       </c>
       <c r="O28">
         <f t="shared" si="7"/>
-        <v>18256.270422535214</v>
+        <v>18059.988732394366</v>
       </c>
       <c r="P28">
         <f t="shared" si="4"/>
@@ -6827,7 +6827,7 @@
       </c>
       <c r="O29">
         <f t="shared" si="7"/>
-        <v>18641.457746478874</v>
+        <v>18437.62676056338</v>
       </c>
       <c r="P29">
         <f t="shared" si="4"/>
@@ -6883,7 +6883,7 @@
       </c>
       <c r="O30">
         <f t="shared" si="7"/>
-        <v>19240.045070422537</v>
+        <v>19028.664788732396</v>
       </c>
       <c r="P30">
         <f t="shared" si="4"/>
@@ -6939,7 +6939,7 @@
       </c>
       <c r="O31">
         <f t="shared" si="7"/>
-        <v>19661.432394366198</v>
+        <v>19442.502816901408</v>
       </c>
       <c r="P31">
         <f t="shared" si="4"/>
@@ -6995,7 +6995,7 @@
       </c>
       <c r="O32">
         <f t="shared" si="7"/>
-        <v>20306.419718309859</v>
+        <v>20079.940845070421</v>
       </c>
       <c r="P32">
         <f t="shared" si="4"/>
@@ -7051,7 +7051,7 @@
       </c>
       <c r="O33">
         <f t="shared" si="7"/>
-        <v>20755.80704225352</v>
+        <v>20521.778873239437</v>
       </c>
       <c r="P33">
         <f t="shared" si="4"/>
@@ -7107,7 +7107,7 @@
       </c>
       <c r="O34">
         <f t="shared" si="7"/>
-        <v>21440.994366197181</v>
+        <v>21199.416901408451</v>
       </c>
       <c r="P34">
         <f t="shared" si="4"/>
@@ -7163,7 +7163,7 @@
       </c>
       <c r="O35">
         <f t="shared" si="9"/>
-        <v>21912.781690140844</v>
+        <v>21663.654929577464</v>
       </c>
       <c r="P35">
         <f t="shared" si="4"/>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="O36">
         <f t="shared" si="9"/>
-        <v>22636.369014084506</v>
+        <v>22379.69295774648</v>
       </c>
       <c r="P36">
         <f t="shared" si="4"/>
@@ -7275,7 +7275,7 @@
       </c>
       <c r="O37">
         <f t="shared" si="9"/>
-        <v>23136.356338028167</v>
+        <v>22872.130985915494</v>
       </c>
       <c r="P37">
         <f t="shared" si="4"/>
@@ -7331,7 +7331,7 @@
       </c>
       <c r="O38">
         <f t="shared" si="9"/>
-        <v>23895.343661971834</v>
+        <v>23623.569014084507</v>
       </c>
       <c r="P38">
         <f t="shared" si="4"/>
@@ -7387,7 +7387,7 @@
       </c>
       <c r="O39">
         <f t="shared" si="9"/>
-        <v>24418.530985915495</v>
+        <v>24139.207042253522</v>
       </c>
       <c r="P39">
         <f t="shared" si="4"/>
@@ -7443,7 +7443,7 @@
       </c>
       <c r="O40">
         <f t="shared" si="9"/>
-        <v>25215.118309859157</v>
+        <v>24928.245070422538</v>
       </c>
       <c r="P40">
         <f t="shared" si="4"/>
@@ -7499,7 +7499,7 @@
       </c>
       <c r="O41">
         <f t="shared" si="9"/>
-        <v>25759.905633802817</v>
+        <v>25465.483098591547</v>
       </c>
       <c r="P41">
         <f t="shared" si="4"/>
@@ -7555,7 +7555,7 @@
       </c>
       <c r="O42">
         <f t="shared" si="9"/>
-        <v>26869.492957746479</v>
+        <v>26567.521126760563</v>
       </c>
       <c r="P42">
         <f t="shared" si="4"/>
@@ -7611,7 +7611,7 @@
       </c>
       <c r="O43">
         <f t="shared" si="9"/>
-        <v>27720.080281690141</v>
+        <v>27410.559154929579</v>
       </c>
       <c r="P43">
         <f t="shared" si="4"/>
@@ -7667,7 +7667,7 @@
       </c>
       <c r="O44">
         <f t="shared" si="9"/>
-        <v>28570.667605633804</v>
+        <v>28253.597183098595</v>
       </c>
       <c r="P44">
         <f t="shared" si="4"/>
@@ -7723,7 +7723,7 @@
       </c>
       <c r="O45">
         <f t="shared" si="9"/>
-        <v>29440.054929577465</v>
+        <v>29115.435211267606</v>
       </c>
       <c r="P45">
         <f t="shared" si="4"/>
@@ -7779,7 +7779,7 @@
       </c>
       <c r="O46">
         <f t="shared" si="9"/>
-        <v>30309.442253521127</v>
+        <v>29977.273239436621</v>
       </c>
       <c r="P46">
         <f t="shared" si="4"/>
@@ -7835,7 +7835,7 @@
       </c>
       <c r="O47">
         <f t="shared" si="9"/>
-        <v>30915.629577464788</v>
+        <v>30575.911267605636</v>
       </c>
       <c r="P47">
         <f t="shared" si="4"/>
@@ -7891,7 +7891,7 @@
       </c>
       <c r="O48">
         <f t="shared" si="9"/>
-        <v>31521.816901408452</v>
+        <v>31174.549295774646</v>
       </c>
       <c r="P48">
         <f t="shared" si="4"/>
@@ -7947,7 +7947,7 @@
       </c>
       <c r="O49">
         <f t="shared" si="9"/>
-        <v>32434.004225352117</v>
+        <v>32079.187323943665</v>
       </c>
       <c r="P49">
         <f t="shared" si="4"/>
@@ -8003,7 +8003,7 @@
       </c>
       <c r="O50">
         <f t="shared" si="9"/>
-        <v>33053.991549295773</v>
+        <v>32691.625352112678</v>
       </c>
       <c r="P50">
         <f t="shared" si="4"/>
@@ -8059,7 +8059,7 @@
       </c>
       <c r="O51">
         <f t="shared" si="11"/>
-        <v>33982.978873239437</v>
+        <v>33613.063380281688</v>
       </c>
       <c r="P51">
         <f t="shared" si="4"/>
@@ -8115,7 +8115,7 @@
       </c>
       <c r="O52">
         <f t="shared" si="11"/>
-        <v>34610.366197183095</v>
+        <v>34232.901408450707</v>
       </c>
       <c r="P52">
         <f t="shared" si="4"/>
@@ -8171,7 +8171,7 @@
       </c>
       <c r="O53">
         <f t="shared" si="11"/>
-        <v>35543.553521126763</v>
+        <v>35158.539436619722</v>
       </c>
       <c r="P53">
         <f t="shared" si="4"/>
@@ -8227,7 +8227,7 @@
       </c>
       <c r="O54">
         <f t="shared" si="11"/>
-        <v>36170.740845070424</v>
+        <v>35778.177464788729</v>
       </c>
       <c r="P54">
         <f t="shared" si="4"/>
@@ -8283,7 +8283,7 @@
       </c>
       <c r="O55">
         <f t="shared" si="11"/>
-        <v>37102.128169014082</v>
+        <v>36702.015492957747</v>
       </c>
       <c r="P55">
         <f t="shared" si="4"/>
@@ -8339,7 +8339,7 @@
       </c>
       <c r="O56">
         <f t="shared" si="11"/>
-        <v>37724.515492957747</v>
+        <v>37316.853521126759</v>
       </c>
       <c r="P56">
         <f t="shared" si="4"/>
@@ -8395,7 +8395,7 @@
       </c>
       <c r="O57">
         <f t="shared" si="11"/>
-        <v>38645.902816901405</v>
+        <v>38230.691549295771</v>
       </c>
       <c r="P57">
         <f t="shared" si="4"/>
@@ -8451,7 +8451,7 @@
       </c>
       <c r="O58">
         <f t="shared" si="11"/>
-        <v>39559.890140845069</v>
+        <v>39137.129577464788</v>
       </c>
       <c r="P58">
         <f t="shared" si="4"/>
@@ -8507,7 +8507,7 @@
       </c>
       <c r="O59">
         <f t="shared" si="11"/>
-        <v>40473.877464788733</v>
+        <v>40043.567605633805</v>
       </c>
       <c r="P59">
         <f t="shared" si="4"/>
@@ -8563,7 +8563,7 @@
       </c>
       <c r="O60">
         <f t="shared" si="11"/>
-        <v>41083.664788732392</v>
+        <v>40645.805633802811</v>
       </c>
       <c r="P60">
         <f t="shared" si="4"/>
@@ -8619,7 +8619,7 @@
       </c>
       <c r="O61">
         <f t="shared" si="11"/>
-        <v>41693.452112676052</v>
+        <v>41248.043661971831</v>
       </c>
       <c r="P61">
         <f t="shared" si="4"/>
@@ -8675,7 +8675,7 @@
       </c>
       <c r="O62">
         <f t="shared" si="11"/>
-        <v>42299.63943661972</v>
+        <v>41846.681690140846</v>
       </c>
       <c r="P62">
         <f t="shared" si="4"/>
@@ -8731,7 +8731,7 @@
       </c>
       <c r="O63">
         <f t="shared" si="11"/>
-        <v>42607.426760563387</v>
+        <v>42146.919718309859</v>
       </c>
       <c r="P63">
         <f t="shared" si="4"/>
@@ -8787,7 +8787,7 @@
       </c>
       <c r="O64">
         <f t="shared" si="11"/>
-        <v>43213.014084507042</v>
+        <v>42744.957746478874</v>
       </c>
       <c r="P64">
         <f t="shared" si="4"/>
@@ -8843,7 +8843,7 @@
       </c>
       <c r="O65">
         <f t="shared" si="11"/>
-        <v>43818.601408450704</v>
+        <v>43342.995774647883</v>
       </c>
       <c r="P65">
         <f t="shared" si="4"/>
@@ -8899,7 +8899,7 @@
       </c>
       <c r="O66">
         <f t="shared" si="11"/>
-        <v>44716.588732394368</v>
+        <v>44233.433802816908</v>
       </c>
       <c r="P66">
         <f t="shared" si="4"/>
@@ -8955,7 +8955,7 @@
       </c>
       <c r="O67">
         <f t="shared" si="14"/>
-        <v>45319.17605633803</v>
+        <v>44828.471830985916</v>
       </c>
       <c r="P67">
         <f t="shared" ref="P67:Q111" si="15">J67</f>
@@ -9011,7 +9011,7 @@
       </c>
       <c r="O68">
         <f t="shared" si="14"/>
-        <v>46212.363380281691</v>
+        <v>45714.109859154931</v>
       </c>
       <c r="P68">
         <f t="shared" si="15"/>
@@ -9067,7 +9067,7 @@
       </c>
       <c r="O69">
         <f t="shared" si="14"/>
-        <v>46807.750704225356</v>
+        <v>46301.94788732395</v>
       </c>
       <c r="P69">
         <f t="shared" si="15"/>
@@ -9123,7 +9123,7 @@
       </c>
       <c r="O70">
         <f t="shared" si="14"/>
-        <v>47692.538028169009</v>
+        <v>47179.185915492955</v>
       </c>
       <c r="P70">
         <f t="shared" si="15"/>
@@ -9179,7 +9179,7 @@
       </c>
       <c r="O71">
         <f t="shared" si="14"/>
-        <v>48284.925352112674</v>
+        <v>47764.023943661967</v>
       </c>
       <c r="P71">
         <f t="shared" si="15"/>
@@ -9235,7 +9235,7 @@
       </c>
       <c r="O72">
         <f t="shared" si="14"/>
-        <v>49162.512676056336</v>
+        <v>48634.06197183099</v>
       </c>
       <c r="P72">
         <f t="shared" si="15"/>
@@ -9291,7 +9291,7 @@
       </c>
       <c r="O73">
         <f t="shared" si="14"/>
-        <v>49749.5</v>
+        <v>49213.5</v>
       </c>
       <c r="P73">
         <f t="shared" si="15"/>
@@ -9347,7 +9347,7 @@
       </c>
       <c r="O74">
         <f t="shared" si="14"/>
-        <v>50613.087323943662</v>
+        <v>50069.538028169009</v>
       </c>
       <c r="P74">
         <f t="shared" si="15"/>
@@ -9403,7 +9403,7 @@
       </c>
       <c r="O75">
         <f t="shared" si="14"/>
-        <v>51187.274647887323</v>
+        <v>50636.17605633803</v>
       </c>
       <c r="P75">
         <f t="shared" si="15"/>
@@ -9459,7 +9459,7 @@
       </c>
       <c r="O76">
         <f t="shared" si="14"/>
-        <v>52027.661971830988</v>
+        <v>51469.014084507042</v>
       </c>
       <c r="P76">
         <f t="shared" si="15"/>
@@ -9515,7 +9515,7 @@
       </c>
       <c r="O77">
         <f t="shared" si="14"/>
-        <v>52582.849295774649</v>
+        <v>52016.652112676056</v>
       </c>
       <c r="P77">
         <f t="shared" si="15"/>
@@ -9571,7 +9571,7 @@
       </c>
       <c r="O78">
         <f t="shared" si="14"/>
-        <v>53392.636619718309</v>
+        <v>52818.890140845069</v>
       </c>
       <c r="P78">
         <f t="shared" si="15"/>
@@ -9627,7 +9627,7 @@
       </c>
       <c r="O79">
         <f t="shared" si="14"/>
-        <v>53925.82394366197</v>
+        <v>53344.528169014084</v>
       </c>
       <c r="P79">
         <f t="shared" si="15"/>
@@ -9683,7 +9683,7 @@
       </c>
       <c r="O80">
         <f t="shared" si="14"/>
-        <v>54700.811267605633</v>
+        <v>54111.966197183094</v>
       </c>
       <c r="P80">
         <f t="shared" si="15"/>
@@ -9739,7 +9739,7 @@
       </c>
       <c r="O81">
         <f t="shared" si="14"/>
-        <v>55209.598591549293</v>
+        <v>54613.204225352114</v>
       </c>
       <c r="P81">
         <f t="shared" si="15"/>
@@ -9795,7 +9795,7 @@
       </c>
       <c r="O82">
         <f t="shared" si="14"/>
-        <v>55949.585915492957</v>
+        <v>55345.642253521124</v>
       </c>
       <c r="P82">
         <f t="shared" si="15"/>
@@ -9851,7 +9851,7 @@
       </c>
       <c r="O83">
         <f t="shared" si="17"/>
-        <v>56434.973239436615</v>
+        <v>55823.480281690143</v>
       </c>
       <c r="P83">
         <f t="shared" si="15"/>
@@ -9907,7 +9907,7 @@
       </c>
       <c r="O84">
         <f t="shared" si="17"/>
-        <v>56920.36056338028</v>
+        <v>56301.318309859154</v>
       </c>
       <c r="P84">
         <f t="shared" si="15"/>
@@ -9963,7 +9963,7 @@
       </c>
       <c r="O85">
         <f t="shared" si="17"/>
-        <v>57591.747887323945</v>
+        <v>56965.156338028166</v>
       </c>
       <c r="P85">
         <f t="shared" si="15"/>
@@ -10019,7 +10019,7 @@
       </c>
       <c r="O86">
         <f t="shared" si="17"/>
-        <v>58263.135211267603</v>
+        <v>57628.994366197185</v>
       </c>
       <c r="P86">
         <f t="shared" si="15"/>
@@ -10075,7 +10075,7 @@
       </c>
       <c r="O87">
         <f t="shared" si="17"/>
-        <v>58902.722535211273</v>
+        <v>58261.032394366201</v>
       </c>
       <c r="P87">
         <f t="shared" si="15"/>
@@ -10131,7 +10131,7 @@
       </c>
       <c r="O88">
         <f t="shared" si="17"/>
-        <v>59542.309859154928</v>
+        <v>58893.070422535209</v>
       </c>
       <c r="P88">
         <f t="shared" si="15"/>
@@ -10187,7 +10187,7 @@
       </c>
       <c r="O89">
         <f t="shared" si="17"/>
-        <v>60372.697183098593</v>
+        <v>59715.908450704228</v>
       </c>
       <c r="P89">
         <f t="shared" si="15"/>
@@ -10243,7 +10243,7 @@
       </c>
       <c r="O90">
         <f t="shared" si="17"/>
-        <v>60775.284507042248</v>
+        <v>60110.946478873237</v>
       </c>
       <c r="P90">
         <f t="shared" si="15"/>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="O91">
         <f t="shared" si="17"/>
-        <v>61358.271830985919</v>
+        <v>60686.384507042254</v>
       </c>
       <c r="P91">
         <f t="shared" si="15"/>
@@ -10355,7 +10355,7 @@
       </c>
       <c r="O92">
         <f t="shared" si="17"/>
-        <v>61741.859154929574</v>
+        <v>61062.42253521127</v>
       </c>
       <c r="P92">
         <f t="shared" si="15"/>
@@ -10411,7 +10411,7 @@
       </c>
       <c r="O93">
         <f t="shared" si="17"/>
-        <v>62295.046478873242</v>
+        <v>61608.060563380284</v>
       </c>
       <c r="P93">
         <f t="shared" si="15"/>
@@ -10467,7 +10467,7 @@
       </c>
       <c r="O94">
         <f t="shared" si="17"/>
-        <v>62657.433802816908</v>
+        <v>61962.898591549296</v>
       </c>
       <c r="P94">
         <f t="shared" si="15"/>
@@ -10523,7 +10523,7 @@
       </c>
       <c r="O95">
         <f t="shared" si="17"/>
-        <v>63019.821126760566</v>
+        <v>62317.736619718315</v>
       </c>
       <c r="P95">
         <f t="shared" si="15"/>
@@ -10579,7 +10579,7 @@
       </c>
       <c r="O96">
         <f t="shared" si="17"/>
-        <v>63359.208450704231</v>
+        <v>62649.574647887326</v>
       </c>
       <c r="P96">
         <f t="shared" si="15"/>
@@ -10635,7 +10635,7 @@
       </c>
       <c r="O97">
         <f t="shared" si="17"/>
-        <v>63698.595774647889</v>
+        <v>62981.412676056338</v>
       </c>
       <c r="P97">
         <f t="shared" si="15"/>
@@ -10691,7 +10691,7 @@
       </c>
       <c r="O98">
         <f t="shared" si="17"/>
-        <v>64013.983098591554</v>
+        <v>63289.250704225356</v>
       </c>
       <c r="P98">
         <f t="shared" si="15"/>
@@ -10747,7 +10747,7 @@
       </c>
       <c r="O99">
         <f t="shared" si="19"/>
-        <v>64329.370422535212</v>
+        <v>63597.088732394368</v>
       </c>
       <c r="P99">
         <f t="shared" si="15"/>
@@ -10803,7 +10803,7 @@
       </c>
       <c r="O100">
         <f t="shared" si="19"/>
-        <v>64778.957746478874</v>
+        <v>64039.126760563384</v>
       </c>
       <c r="P100">
         <f t="shared" si="15"/>
@@ -10859,7 +10859,7 @@
       </c>
       <c r="O101">
         <f t="shared" si="19"/>
-        <v>65071.145070422535</v>
+        <v>64323.764788732398</v>
       </c>
       <c r="P101">
         <f t="shared" si="15"/>
@@ -10915,7 +10915,7 @@
       </c>
       <c r="O102">
         <f t="shared" si="19"/>
-        <v>65485.932394366195</v>
+        <v>64731.002816901404</v>
       </c>
       <c r="P102">
         <f t="shared" si="15"/>
@@ -10971,7 +10971,7 @@
       </c>
       <c r="O103">
         <f t="shared" si="19"/>
-        <v>65755.119718309856</v>
+        <v>64992.640845070426</v>
       </c>
       <c r="P103">
         <f t="shared" si="15"/>
@@ -11027,7 +11027,7 @@
       </c>
       <c r="O104">
         <f t="shared" si="19"/>
-        <v>66132.507042253521</v>
+        <v>65362.478873239437</v>
       </c>
       <c r="P104">
         <f t="shared" si="15"/>
@@ -11083,7 +11083,7 @@
       </c>
       <c r="O105">
         <f t="shared" si="19"/>
-        <v>66375.694366197189</v>
+        <v>65598.116901408459</v>
       </c>
       <c r="P105">
         <f t="shared" si="15"/>
@@ -11139,7 +11139,7 @@
       </c>
       <c r="O106">
         <f t="shared" si="19"/>
-        <v>66740.481690140849</v>
+        <v>65955.354929577457</v>
       </c>
       <c r="P106">
         <f t="shared" si="15"/>
@@ -11195,7 +11195,7 @@
       </c>
       <c r="O107">
         <f t="shared" si="19"/>
-        <v>66982.669014084502</v>
+        <v>66189.992957746479</v>
       </c>
       <c r="P107">
         <f t="shared" si="15"/>
@@ -11251,7 +11251,7 @@
       </c>
       <c r="O108">
         <f t="shared" si="19"/>
-        <v>67224.85633802817</v>
+        <v>66424.630985915501</v>
       </c>
       <c r="P108">
         <f t="shared" si="15"/>
@@ -11307,7 +11307,7 @@
       </c>
       <c r="O109">
         <f t="shared" si="19"/>
-        <v>67389.043661971838</v>
+        <v>66581.269014084508</v>
       </c>
       <c r="P109">
         <f t="shared" si="15"/>
@@ -11363,7 +11363,7 @@
       </c>
       <c r="O110">
         <f t="shared" si="19"/>
-        <v>67553.230985915492</v>
+        <v>66737.907042253515</v>
       </c>
       <c r="P110">
         <f t="shared" si="15"/>
@@ -11419,7 +11419,7 @@
       </c>
       <c r="O111">
         <f t="shared" si="19"/>
-        <v>67617.418309859146</v>
+        <v>66794.545070422537</v>
       </c>
       <c r="P111">
         <f t="shared" si="15"/>
@@ -11475,7 +11475,7 @@
       </c>
       <c r="O112">
         <f t="shared" ref="O112:O144" si="26">I112+V$9 +($M111*V$10)</f>
-        <v>67681.605633802814</v>
+        <v>66851.183098591544</v>
       </c>
       <c r="P112">
         <f t="shared" ref="P112:P144" si="27">J112</f>
@@ -11531,7 +11531,7 @@
       </c>
       <c r="O113">
         <f t="shared" si="26"/>
-        <v>67759.392957746473</v>
+        <v>66921.421126760557</v>
       </c>
       <c r="P113">
         <f t="shared" si="27"/>
@@ -11587,7 +11587,7 @@
       </c>
       <c r="O114">
         <f t="shared" si="26"/>
-        <v>67806.98028169015</v>
+        <v>66961.459154929587</v>
       </c>
       <c r="P114">
         <f t="shared" si="27"/>
@@ -11643,7 +11643,7 @@
       </c>
       <c r="O115">
         <f t="shared" si="26"/>
-        <v>67861.76760563381</v>
+        <v>67008.697183098586</v>
       </c>
       <c r="P115">
         <f t="shared" si="27"/>
@@ -11699,7 +11699,7 @@
       </c>
       <c r="O116">
         <f t="shared" si="26"/>
-        <v>67894.954929577463</v>
+        <v>67034.335211267608</v>
       </c>
       <c r="P116">
         <f t="shared" si="27"/>
@@ -11755,7 +11755,7 @@
       </c>
       <c r="O117">
         <f t="shared" si="26"/>
-        <v>67931.342253521128</v>
+        <v>67063.173239436626</v>
       </c>
       <c r="P117">
         <f t="shared" si="27"/>
@@ -11811,7 +11811,7 @@
       </c>
       <c r="O118">
         <f t="shared" si="26"/>
-        <v>67954.129577464788</v>
+        <v>67078.411267605625</v>
       </c>
       <c r="P118">
         <f t="shared" si="27"/>
@@ -11867,7 +11867,7 @@
       </c>
       <c r="O119">
         <f t="shared" si="26"/>
-        <v>67973.916901408462</v>
+        <v>67090.649295774652</v>
       </c>
       <c r="P119">
         <f t="shared" si="27"/>
@@ -11923,7 +11923,7 @@
       </c>
       <c r="O120">
         <f t="shared" si="26"/>
-        <v>67986.50422535211</v>
+        <v>67095.687323943668</v>
       </c>
       <c r="P120">
         <f t="shared" si="27"/>
@@ -11979,7 +11979,7 @@
       </c>
       <c r="O121">
         <f t="shared" si="26"/>
-        <v>67996.891549295775</v>
+        <v>67098.525352112672</v>
       </c>
       <c r="P121">
         <f t="shared" si="27"/>
@@ -12035,7 +12035,7 @@
       </c>
       <c r="O122">
         <f t="shared" si="26"/>
-        <v>68004.078873239443</v>
+        <v>67098.163380281694</v>
       </c>
       <c r="P122">
         <f t="shared" si="27"/>
@@ -12091,7 +12091,7 @@
       </c>
       <c r="O123">
         <f t="shared" si="26"/>
-        <v>68003.666197183105</v>
+        <v>67090.20140845071</v>
       </c>
       <c r="P123">
         <f t="shared" si="27"/>
@@ -12147,7 +12147,7 @@
       </c>
       <c r="O124">
         <f t="shared" si="26"/>
-        <v>68006.253521126768</v>
+        <v>67085.239436619711</v>
       </c>
       <c r="P124">
         <f t="shared" si="27"/>
@@ -12203,7 +12203,7 @@
       </c>
       <c r="O125">
         <f t="shared" si="26"/>
-        <v>67995.040845070413</v>
+        <v>67066.477464788724</v>
       </c>
       <c r="P125">
         <f t="shared" si="27"/>
@@ -12259,7 +12259,7 @@
       </c>
       <c r="O126">
         <f t="shared" si="26"/>
-        <v>67986.028169014084</v>
+        <v>67049.915492957749</v>
       </c>
       <c r="P126">
         <f t="shared" si="27"/>
@@ -12315,7 +12315,7 @@
       </c>
       <c r="O127">
         <f t="shared" si="26"/>
-        <v>67968.615492957746</v>
+        <v>67024.953521126765</v>
       </c>
       <c r="P127">
         <f t="shared" si="27"/>
@@ -12371,7 +12371,7 @@
       </c>
       <c r="O128">
         <f t="shared" si="26"/>
-        <v>67958.802816901414</v>
+        <v>67007.591549295772</v>
       </c>
       <c r="P128">
         <f t="shared" si="27"/>
@@ -12427,7 +12427,7 @@
       </c>
       <c r="O129">
         <f t="shared" si="26"/>
-        <v>67946.590140845059</v>
+        <v>66987.829577464785</v>
       </c>
       <c r="P129">
         <f t="shared" si="27"/>
@@ -12483,7 +12483,7 @@
       </c>
       <c r="O130">
         <f t="shared" si="26"/>
-        <v>67948.177464788736</v>
+        <v>66981.867605633815</v>
       </c>
       <c r="P130">
         <f t="shared" si="27"/>
@@ -12539,7 +12539,7 @@
       </c>
       <c r="O131">
         <f t="shared" si="26"/>
-        <v>67952.164788732392</v>
+        <v>66978.305633802811</v>
       </c>
       <c r="P131">
         <f t="shared" si="27"/>
@@ -12595,7 +12595,7 @@
       </c>
       <c r="O132">
         <f t="shared" si="26"/>
-        <v>67964.552112676058</v>
+        <v>66983.14366197183</v>
       </c>
       <c r="P132">
         <f t="shared" si="27"/>
@@ -12651,7 +12651,7 @@
       </c>
       <c r="O133">
         <f t="shared" si="26"/>
-        <v>67975.139436619706</v>
+        <v>66986.181690140846</v>
       </c>
       <c r="P133">
         <f t="shared" si="27"/>
@@ -12707,7 +12707,7 @@
       </c>
       <c r="O134">
         <f t="shared" si="26"/>
-        <v>67988.126760563377</v>
+        <v>66991.619718309856</v>
       </c>
       <c r="P134">
         <f t="shared" si="27"/>
@@ -12763,7 +12763,7 @@
       </c>
       <c r="O135">
         <f t="shared" si="26"/>
-        <v>67999.114084507048</v>
+        <v>66995.05774647888</v>
       </c>
       <c r="P135">
         <f t="shared" si="27"/>
@@ -12819,7 +12819,7 @@
       </c>
       <c r="O136">
         <f t="shared" si="26"/>
-        <v>68007.70140845071</v>
+        <v>66996.095774647896</v>
       </c>
       <c r="P136">
         <f t="shared" si="27"/>
@@ -12875,7 +12875,7 @@
       </c>
       <c r="O137">
         <f t="shared" si="26"/>
-        <v>68012.088732394375</v>
+        <v>66992.9338028169</v>
       </c>
       <c r="P137">
         <f t="shared" si="27"/>
@@ -12931,7 +12931,7 @@
       </c>
       <c r="O138">
         <f t="shared" si="26"/>
-        <v>68018.276056338029</v>
+        <v>66991.571830985922</v>
       </c>
       <c r="P138">
         <f t="shared" si="27"/>
@@ -12987,7 +12987,7 @@
       </c>
       <c r="O139">
         <f t="shared" si="26"/>
-        <v>68015.663380281694</v>
+        <v>66981.409859154941</v>
       </c>
       <c r="P139">
         <f t="shared" si="27"/>
@@ -13043,7 +13043,7 @@
       </c>
       <c r="O140">
         <f t="shared" si="26"/>
-        <v>68015.050704225359</v>
+        <v>66973.247887323945</v>
       </c>
       <c r="P140">
         <f t="shared" si="27"/>
@@ -13099,7 +13099,7 @@
       </c>
       <c r="O141">
         <f t="shared" si="26"/>
-        <v>68007.638028169022</v>
+        <v>66958.285915492961</v>
       </c>
       <c r="P141">
         <f t="shared" si="27"/>
@@ -13155,7 +13155,7 @@
       </c>
       <c r="O142">
         <f t="shared" si="26"/>
-        <v>68004.425352112667</v>
+        <v>66947.523943661974</v>
       </c>
       <c r="P142">
         <f t="shared" si="27"/>
@@ -13211,7 +13211,7 @@
       </c>
       <c r="O143">
         <f t="shared" si="26"/>
-        <v>67998.946009389663</v>
+        <v>66934.49530516431</v>
       </c>
       <c r="P143">
         <f t="shared" si="27"/>
@@ -13267,7 +13267,7 @@
       </c>
       <c r="O144">
         <f t="shared" si="26"/>
-        <v>68000</v>
+        <v>66928</v>
       </c>
       <c r="P144">
         <f t="shared" si="27"/>
@@ -14271,8 +14271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3ECCBA-6D4F-466F-804D-502AE8BB8A06}">
   <dimension ref="A1:V331"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:R1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>